<commit_message>
atualizações do ZIP + fix Live Server no export PDF
</commit_message>
<xml_diff>
--- a/DASHBOARD.xlsx
+++ b/DASHBOARD.xlsx
@@ -1478,19 +1478,17 @@
         <f>IF(AND(E13="READY",F13="No",G13="Yes",H13="Yes"),"Yes","No")</f>
         <v/>
       </c>
-      <c r="L13" s="10" t="inlineStr">
-        <is>
-          <t>2026-01-22</t>
-        </is>
+      <c r="L13" s="10" t="n">
+        <v>46044</v>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>P1: adicionar/confirmar referências (CAC, eventos, follow-up)</t>
+          <t>P1: inserir HR/IC do seguimento 10 anos + figura (paper pendente)</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>Batch 06–15: contraste/hierarquia + cards GRADE em layout claro; utilitários .card/.chip. | Patch 2.1: contraste chips em header navy + S09 source strip</t>
+          <t>Placeholders adicionados (10y HR/CI + figura/citação). Mantém dados atuais (4.7y) até atualização.</t>
         </is>
       </c>
     </row>
@@ -1724,7 +1722,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>DRAFT</t>
+          <t>READY</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1734,18 +1732,21 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
+      </c>
+      <c r="J17" t="n">
+        <v>9</v>
       </c>
       <c r="K17">
         <f>IF(AND(E17="READY",F17="No",G17="Yes",H17="Yes"),"Yes","No")</f>
@@ -1756,7 +1757,12 @@
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>P1: revisar evidência (bempedoic/SAMS) + rodapé</t>
+          <t>P2: revisão final de texto (aula/residentes)</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>Batch 16–26: layout ok, sem overflow.</t>
         </is>
       </c>
     </row>
@@ -1783,7 +1789,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>DRAFT</t>
+          <t>READY</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1793,18 +1799,21 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
+      </c>
+      <c r="J18" t="n">
+        <v>9</v>
       </c>
       <c r="K18">
         <f>IF(AND(E18="READY",F18="No",G18="Yes",H18="Yes"),"Yes","No")</f>
@@ -1815,7 +1824,12 @@
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>P1: revisar MID/imprecisão + CLEAR Outcomes</t>
+          <t>P2: checar legibilidade da barra MID em projetor</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>Batch 16–26: padronizado.</t>
         </is>
       </c>
     </row>
@@ -1842,7 +1856,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>DRAFT</t>
+          <t>READY</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1852,18 +1866,21 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
+      </c>
+      <c r="J19" t="n">
+        <v>9</v>
       </c>
       <c r="K19">
         <f>IF(AND(E19="READY",F19="No",G19="Yes",H19="Yes"),"Yes","No")</f>
@@ -1874,12 +1891,12 @@
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>P1: revisar MID/imprecisão + CLEAR Outcomes</t>
+          <t>P2: revisar texto 'rebaxar -1 nível'</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>P0: conteúdo invisível por cor/opacity (ver METRICAS_MVP.txt).</t>
+          <t>Batch 16–26: compactado.</t>
         </is>
       </c>
     </row>
@@ -1906,7 +1923,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>DRAFT</t>
+          <t>READY</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1916,18 +1933,21 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
+      </c>
+      <c r="J20" t="n">
+        <v>9</v>
       </c>
       <c r="K20">
         <f>IF(AND(E20="READY",F20="No",G20="Yes",H20="Yes"),"Yes","No")</f>
@@ -1938,7 +1958,12 @@
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>P1: alinhar com RoB/EtD oficiais + exemplos</t>
+          <t>P2: validar se 5 domínios RoB2 cabem em telas menores</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>Compactação de paddings/font para evitar corte do item 5.</t>
         </is>
       </c>
     </row>
@@ -1965,7 +1990,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>DRAFT</t>
+          <t>READY</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1975,18 +2000,21 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
+      </c>
+      <c r="J21" t="n">
+        <v>9</v>
       </c>
       <c r="K21">
         <f>IF(AND(E21="READY",F21="No",G21="Yes",H21="Yes"),"Yes","No")</f>
@@ -1997,7 +2025,12 @@
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>P1: alinhar com RoB/EtD oficiais + exemplos</t>
+          <t>P2: checar contraste da linha RECOMENDAÇÃO no projetor</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>Tabela EtD revisada; recomendação destacada.</t>
         </is>
       </c>
     </row>
@@ -2142,7 +2175,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>DRAFT</t>
+          <t>READY</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2152,18 +2185,21 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
+      </c>
+      <c r="J24" t="n">
+        <v>9</v>
       </c>
       <c r="K24">
         <f>IF(AND(E24="READY",F24="No",G24="Yes",H24="Yes"),"Yes","No")</f>
@@ -2174,7 +2210,12 @@
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>P1: validar métricas PREVENT/prognóstico + fontes</t>
+          <t>P2: revisar mensagem sobre validação BR (sem datas)</t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>Fonte corrigida para Circulation 2024 PREVENT; removido '2026'.</t>
         </is>
       </c>
     </row>
@@ -2201,7 +2242,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>DRAFT</t>
+          <t>READY</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2211,18 +2252,21 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
+      </c>
+      <c r="J25" t="n">
+        <v>9</v>
       </c>
       <c r="K25">
         <f>IF(AND(E25="READY",F25="No",G25="Yes",H25="Yes"),"Yes","No")</f>
@@ -2233,7 +2277,12 @@
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>P1: validar métricas PREVENT/prognóstico + fontes</t>
+          <t>P2: validar narrativa 10y vs 30y</t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>Fontes corrigidas (PREVENT Circulation 2024 + Framingham 30y Circulation 2009).</t>
         </is>
       </c>
     </row>
@@ -2260,7 +2309,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>DRAFT</t>
+          <t>READY</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2270,18 +2319,21 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
+      </c>
+      <c r="J26" t="n">
+        <v>9</v>
       </c>
       <c r="K26">
         <f>IF(AND(E26="READY",F26="No",G26="Yes",H26="Yes"),"Yes","No")</f>
@@ -2292,7 +2344,12 @@
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>P1: validar tabelas (calculadoras, PROBAST, TRIPOD+AI)</t>
+          <t>P2: revisão final da tabela comparativa</t>
+        </is>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>Fontes corrigidas (PREVENT, PCE guideline, SCORE2). Mensagem-chave mais cautelosa.</t>
         </is>
       </c>
     </row>
@@ -3263,7 +3320,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>DRAFT</t>
+          <t>READY</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3273,18 +3330,21 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
+      </c>
+      <c r="J43" t="n">
+        <v>9</v>
       </c>
       <c r="K43">
         <f>IF(AND(E43="READY",F43="No",G43="Yes",H43="Yes"),"Yes","No")</f>
@@ -3295,7 +3355,12 @@
       </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>P1: revisão final de síntese + consistência de termos</t>
+          <t>P2: checar contraste do painel escuro em projetor</t>
+        </is>
+      </c>
+      <c r="N43" t="inlineStr">
+        <is>
+          <t>Fix: texto ilegível no navy (Rabdomiólise/contraindicação).</t>
         </is>
       </c>
     </row>
@@ -3440,7 +3505,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>DRAFT</t>
+          <t>READY</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3450,18 +3515,21 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
         <is>
           <t>Low</t>
         </is>
+      </c>
+      <c r="J46" t="n">
+        <v>9</v>
       </c>
       <c r="K46">
         <f>IF(AND(E46="READY",F46="No",G46="Yes",H46="Yes"),"Yes","No")</f>
@@ -3472,12 +3540,12 @@
       </c>
       <c r="M46" t="inlineStr">
         <is>
-          <t>P1: revisão final de síntese + consistência de termos</t>
+          <t>P2: checar contraste do painel BR em projetor</t>
         </is>
       </c>
       <c r="N46" t="inlineStr">
         <is>
-          <t>Adicionado: existia no código (S46.html), faltava no dashboard.</t>
+          <t>Fix: 'PCSK9i indisponível no SUS' agora em vermelho legível no navy.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: .html no fetch dos slides (_list.txt) + ver-local, slides S50-S59, CSS e demais
</commit_message>
<xml_diff>
--- a/DASHBOARD.xlsx
+++ b/DASHBOARD.xlsx
@@ -329,7 +329,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,7 +424,7 @@
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t>Placeholder</t>
+          <t>Atualizado</t>
         </is>
       </c>
       <c r="F2" s="3" t="inlineStr">
@@ -434,22 +434,22 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>2026-01-23</t>
+          <t>2026-01-25</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
         <is>
-          <t>Atualizado com números SCOT-HEART 10y (Lancet 2025) + padding/altura; figura ainda placeholder</t>
+          <t>Figura incluída (KM esquemático) + citação SCOT-HEART 10y corrigida; padding ajustado.</t>
         </is>
       </c>
       <c r="I2" s="2" t="inlineStr">
         <is>
-          <t>Lancet 2025 (SCOT-HEART 10y); Circulation 2020 (LAP)</t>
+          <t>Lancet 2025 (SCOT-HEART 10y; 10.1016/S0140-6736(24)01899-5); Circulation 2020 (LAP)</t>
         </is>
       </c>
       <c r="J2" s="2" t="inlineStr">
         <is>
-          <t>Inserir figura (Kaplan–Meier) com citação completa</t>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -1206,7 +1206,32 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>DONE</t>
+          <t>Atualizado</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Título sem destaque em dourado; tipografia alinhada ao padrão.</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>PREVENT/validações externas (referências no slide)</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -1234,6 +1259,526 @@
       <c r="E19" t="inlineStr">
         <is>
           <t>DONE</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>GRADE</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>S50</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Metas lipídicas (abertura)</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Metas</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Novo</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>P0</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Slide de abertura do bloco de metas (SBC 2025)</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>SBC 2025 (10.36660/abc.20250640)</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>GRADE</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>S51</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Metas por categoria de risco (LDL/não-HDL/ApoB)</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Metas</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Novo</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>P0</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Tabela-resumo com alvos e notas práticas</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>SBC 2025 (Tabela 3.1; 10.36660/abc.20250640)</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>GRADE</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>S52</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Força e certeza das metas (conexão com GRADE)</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Metas</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Novo</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>P0</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Tabela força/certeza + explicação por domínios/EtD</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>SBC 2025 (GRADE)</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>GRADE</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>S53</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Base de evidência: CTT + trials + atualização (VESALIUS-CV)</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Metas</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Novo</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>P0</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Resumo fundação + trials + 'living evidence'</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>SBC 2025 refs; NEJMoa2514428</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>GRADE</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>S54</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Inconsistência: quando rebaixar?</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Core GRADE</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Novo</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>P0</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Slide didático de inconsistência (outlier/explicação)</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>BMJ Core GRADE 3 (10.1136/bmj-2024-081905)</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>GRADE</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>S55</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Viés de publicação: como suspeitar?</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Core GRADE</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Novo</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>P0</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Sinais e ações práticas no GRADE</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>BMJ Core GRADE 4 (10.1136/bmj-2024-083864)</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>GRADE</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>S56</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Divergências entre diretrizes (alto nível)</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Metas</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Novo</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Tabela comparativa SBC vs ESC/EAS vs ACC vs AACE</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>SBC 2025; ESC/EAS 2019; ACC ECDP 2022; AACE visual guide</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>GRADE</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>S57</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Take-home: meta é decisão (EtD)</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Metas</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Novo</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>P0</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>Fechamento do bloco + ponte para apêndice</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>SBC 2025 + GRADE/EtD</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>GRADE</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>S58</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Apêndice (divisor)</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Apêndice</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Novo</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Slide divisor para manter PREVENT/CAC no fim</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>GRADE</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>S59</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Encerramento com poesia (Camões)</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Fechamento</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Novo</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Slide final (domínio público)</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>Camões (domínio público)</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fix(GRADE): .html no fetch (_list.txt) em slides-simple, defaultSlideIds/next/prev, slides e CSS
</commit_message>
<xml_diff>
--- a/DASHBOARD.xlsx
+++ b/DASHBOARD.xlsx
@@ -329,7 +329,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,7 +439,7 @@
       </c>
       <c r="H2" s="2" t="inlineStr">
         <is>
-          <t>Figura incluída (KM esquemático) + citação SCOT-HEART 10y corrigida; padding ajustado.</t>
+          <t>Ajustes finos de padding/spacing para evitar corte; compactação de blocos e rodapé.</t>
         </is>
       </c>
       <c r="I2" s="2" t="inlineStr">
@@ -449,7 +449,7 @@
       </c>
       <c r="J2" s="2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>—</t>
         </is>
       </c>
     </row>
@@ -1001,17 +1001,17 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>P0</t>
+          <t>P1</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>2026-01-23</t>
+          <t>2026-01-25</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Revisão de consistência visual (mantido layout); segue como base para downgrade por imprecisão</t>
+          <t>Marcador de IC 95% redesenhado (mais limpo) + ajustes visuais menores.</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -1021,7 +1021,7 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>—</t>
         </is>
       </c>
     </row>
@@ -1053,17 +1053,17 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>P0</t>
+          <t>P1</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>2026-01-23</t>
+          <t>2026-01-25</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Decisão final sem emoji; selo ✓ consistente (navy/teal)</t>
+          <t>Tabela passou a usar estilo global table-medium (padding consistente).</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1073,7 +1073,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>—</t>
         </is>
       </c>
     </row>
@@ -1152,7 +1152,32 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>DONE</t>
+          <t>Atualizado</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Redesign completo + conteúdo (TRIPOD/PROBAST, discriminação vs calibração, validação).</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>TRIPOD/PROBAST</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>—</t>
         </is>
       </c>
     </row>
@@ -1211,7 +1236,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>P2</t>
+          <t>P1</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -1221,7 +1246,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Título sem destaque em dourado; tipografia alinhada ao padrão.</t>
+          <t>Ajuste de paleta do card “Conceito” (header navy + chip gold) + ref PREVENT/PCE.</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -1231,7 +1256,7 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>—</t>
         </is>
       </c>
     </row>
@@ -1337,7 +1362,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Novo</t>
+          <t>Atualizado</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1352,7 +1377,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Tabela-resumo com alvos e notas práticas</t>
+          <t>Tabela ipsis litteris (Extremo) + chip “novo” e nota em rodapé.</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -1362,7 +1387,7 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>—</t>
         </is>
       </c>
     </row>
@@ -1441,12 +1466,12 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Novo</t>
+          <t>Atualizado</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>P0</t>
+          <t>P1</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -1456,7 +1481,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Resumo fundação + trials + 'living evidence'</t>
+          <t>Atualização VESALIUS‑CV: inclusão de HR/IC (3‑point e 4‑point MACE).</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -1466,7 +1491,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>—</t>
         </is>
       </c>
     </row>
@@ -1545,12 +1570,12 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Novo</t>
+          <t>Atualizado</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>P0</t>
+          <t>P1</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -1560,7 +1585,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Sinais e ações práticas no GRADE</t>
+          <t>Incluído lembrete “rate up” (Core GRADE) no contexto de viés de publicação.</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -1570,7 +1595,7 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>—</t>
         </is>
       </c>
     </row>
@@ -1597,7 +1622,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Novo</t>
+          <t>Atualizado</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1612,7 +1637,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Tabela comparativa SBC vs ESC/EAS vs ACC vs AACE</t>
+          <t>Linha AACE 2025 ajustada (meta LDL&lt;70 + recomendações farmacológicas) + refs completas.</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -1622,7 +1647,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>—</t>
         </is>
       </c>
     </row>
@@ -1779,6 +1804,110 @@
       <c r="J29" t="inlineStr">
         <is>
           <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>GRADE</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>S08</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Certeza da evidência (GRADE): domínio–resposta</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Fundamentos</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Atualizado</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Ajuste de paleta (remoção de teal residual), alinhamento/spacing e padronização visual.</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>Core GRADE (visão geral)</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>GRADE</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>S22</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Diretrizes: calculadoras de risco &amp; papel do CAC</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Apêndice (PREVENT)</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Atualizado</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Redesign completo (cards consistentes) + fontes e mensagem-chave (EtD).</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>SBC 2025; ACC/AHA 2019; ESC 2021</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>—</t>
         </is>
       </c>
     </row>
@@ -1793,7 +1922,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1911,6 +2040,33 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Patch 2.7</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>P0/P1: navegação e ordem (main→metas→encerramento→apêndice); ajustes de paleta/padding; redesign PREVENT (S22–S23); atualização refs (AACE 2025, VESALIUS‑CV).</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>ZIP com arquivos modificados (HTML/CSS/JS + DASHBOARD + CHANGELOG).</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Nav sem loop; h2 padronizado (2.85vw); table-medium; S51 ipsis litteris (Extremo).</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
chore: OSTEOPOROSE print.html, print/viewer.css, viewer.js, slides, CHANGELOG, README, DASHBOARD
</commit_message>
<xml_diff>
--- a/DASHBOARD.xlsx
+++ b/DASHBOARD.xlsx
@@ -329,7 +329,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,7 +439,7 @@
       </c>
       <c r="H2" s="2" t="inlineStr">
         <is>
-          <t>Ajustes finos de padding/spacing para evitar corte; compactação de blocos e rodapé.</t>
+          <t>Figura incluída (KM esquemático) + citação SCOT-HEART 10y corrigida; padding ajustado.</t>
         </is>
       </c>
       <c r="I2" s="2" t="inlineStr">
@@ -449,7 +449,7 @@
       </c>
       <c r="J2" s="2" t="inlineStr">
         <is>
-          <t>—</t>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -1001,17 +1001,17 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>P1</t>
+          <t>P0</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>2026-01-25</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Marcador de IC 95% redesenhado (mais limpo) + ajustes visuais menores.</t>
+          <t>Revisão de consistência visual (mantido layout); segue como base para downgrade por imprecisão</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -1021,7 +1021,7 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>—</t>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -1053,17 +1053,17 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>P1</t>
+          <t>P0</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>2026-01-25</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Tabela passou a usar estilo global table-medium (padding consistente).</t>
+          <t>Decisão final sem emoji; selo ✓ consistente (navy/teal)</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1073,7 +1073,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>—</t>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -1152,32 +1152,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Atualizado</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>P2</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>2026-01-25</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>Redesign completo + conteúdo (TRIPOD/PROBAST, discriminação vs calibração, validação).</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>TRIPOD/PROBAST</t>
-        </is>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>—</t>
+          <t>DONE</t>
         </is>
       </c>
     </row>
@@ -1236,7 +1211,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>P1</t>
+          <t>P2</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -1246,7 +1221,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Ajuste de paleta do card “Conceito” (header navy + chip gold) + ref PREVENT/PCE.</t>
+          <t>Título sem destaque em dourado; tipografia alinhada ao padrão.</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -1256,7 +1231,7 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>—</t>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -1362,7 +1337,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Atualizado</t>
+          <t>Novo</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1377,7 +1352,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Tabela ipsis litteris (Extremo) + chip “novo” e nota em rodapé.</t>
+          <t>Tabela-resumo com alvos e notas práticas</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -1387,7 +1362,7 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>—</t>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -1466,12 +1441,12 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Atualizado</t>
+          <t>Novo</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>P1</t>
+          <t>P0</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -1481,7 +1456,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Atualização VESALIUS‑CV: inclusão de HR/IC (3‑point e 4‑point MACE).</t>
+          <t>Resumo fundação + trials + 'living evidence'</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -1491,7 +1466,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>—</t>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -1570,12 +1545,12 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Atualizado</t>
+          <t>Novo</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>P1</t>
+          <t>P0</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -1585,7 +1560,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Incluído lembrete “rate up” (Core GRADE) no contexto de viés de publicação.</t>
+          <t>Sinais e ações práticas no GRADE</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -1595,7 +1570,7 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>—</t>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -1622,7 +1597,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Atualizado</t>
+          <t>Novo</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1637,7 +1612,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Linha AACE 2025 ajustada (meta LDL&lt;70 + recomendações farmacológicas) + refs completas.</t>
+          <t>Tabela comparativa SBC vs ESC/EAS vs ACC vs AACE</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -1647,7 +1622,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>—</t>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -1804,110 +1779,6 @@
       <c r="J29" t="inlineStr">
         <is>
           <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>GRADE</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>S08</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>Certeza da evidência (GRADE): domínio–resposta</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>Fundamentos</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>Atualizado</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>P1</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>2026-01-25</t>
-        </is>
-      </c>
-      <c r="H30" t="inlineStr">
-        <is>
-          <t>Ajuste de paleta (remoção de teal residual), alinhamento/spacing e padronização visual.</t>
-        </is>
-      </c>
-      <c r="I30" t="inlineStr">
-        <is>
-          <t>Core GRADE (visão geral)</t>
-        </is>
-      </c>
-      <c r="J30" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>GRADE</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>S22</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>Diretrizes: calculadoras de risco &amp; papel do CAC</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>Apêndice (PREVENT)</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>Atualizado</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>P2</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>2026-01-25</t>
-        </is>
-      </c>
-      <c r="H31" t="inlineStr">
-        <is>
-          <t>Redesign completo (cards consistentes) + fontes e mensagem-chave (EtD).</t>
-        </is>
-      </c>
-      <c r="I31" t="inlineStr">
-        <is>
-          <t>SBC 2025; ACC/AHA 2019; ESC 2021</t>
-        </is>
-      </c>
-      <c r="J31" t="inlineStr">
-        <is>
-          <t>—</t>
         </is>
       </c>
     </row>
@@ -1922,7 +1793,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2040,33 +1911,6 @@
         </is>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2026-01-25</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Patch 2.7</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>P0/P1: navegação e ordem (main→metas→encerramento→apêndice); ajustes de paleta/padding; redesign PREVENT (S22–S23); atualização refs (AACE 2025, VESALIUS‑CV).</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>ZIP com arquivos modificados (HTML/CSS/JS + DASHBOARD + CHANGELOG).</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Nav sem loop; h2 padronizado (2.85vw); table-medium; S51 ipsis litteris (Extremo).</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
TREE.md, GRADE: slides S60/S61, ajustes S12/S47, _list, figure, CHANGELOG, DASHBOARD
</commit_message>
<xml_diff>
--- a/DASHBOARD.xlsx
+++ b/DASHBOARD.xlsx
@@ -329,7 +329,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -429,7 +429,7 @@
       </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>P1</t>
+          <t>P0</t>
         </is>
       </c>
       <c r="G2" s="2" t="inlineStr">
@@ -439,12 +439,12 @@
       </c>
       <c r="H2" s="2" t="inlineStr">
         <is>
-          <t>Figura incluída (KM esquemático) + citação SCOT-HEART 10y corrigida; padding ajustado.</t>
+          <t>Cards inferiores em paralelo + rodapé absoluto; placeholder KM (esquemático) pronto para substituir pela figura do paper.</t>
         </is>
       </c>
       <c r="I2" s="2" t="inlineStr">
         <is>
-          <t>Lancet 2025 (SCOT-HEART 10y; 10.1016/S0140-6736(24)01899-5); Circulation 2020 (LAP)</t>
+          <t>Lancet 2025 (SCOT-HEART 10y; 10.1016/S0140-6736(24)02679-5; CC BY 4.0); Circulation 2020 (LAP)</t>
         </is>
       </c>
       <c r="J2" s="2" t="inlineStr">
@@ -684,7 +684,7 @@
       </c>
       <c r="E7" s="3" t="inlineStr">
         <is>
-          <t>Reposicionado</t>
+          <t>Atualizado</t>
         </is>
       </c>
       <c r="F7" s="3" t="inlineStr">
@@ -694,17 +694,17 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>2026-01-23</t>
+          <t>2026-01-25</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
         <is>
-          <t>Mantido conteúdo; reposicionado como ponte para EtD</t>
+          <t>Reservado espaço inferior + rodapé absoluto (evita corte em projeção).</t>
         </is>
       </c>
       <c r="I7" s="2" t="inlineStr">
         <is>
-          <t>NEJM 2023 (CLEAR Outcomes)</t>
+          <t>NEJM 2023 (CLEAR Outcomes; 10.1056/NEJMoa2215024)</t>
         </is>
       </c>
       <c r="J7" s="2" t="inlineStr">
@@ -1777,6 +1777,110 @@
         </is>
       </c>
       <c r="J29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="inlineStr">
+        <is>
+          <t>GRADE</t>
+        </is>
+      </c>
+      <c r="B30" s="2" t="inlineStr">
+        <is>
+          <t>S60</t>
+        </is>
+      </c>
+      <c r="C30" s="2" t="inlineStr">
+        <is>
+          <t>Abertura do bloco CAC</t>
+        </is>
+      </c>
+      <c r="D30" s="2" t="inlineStr">
+        <is>
+          <t>CAC / Evidência</t>
+        </is>
+      </c>
+      <c r="E30" s="3" t="inlineStr">
+        <is>
+          <t>Novo</t>
+        </is>
+      </c>
+      <c r="F30" s="3" t="inlineStr">
+        <is>
+          <t>P0</t>
+        </is>
+      </c>
+      <c r="G30" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="H30" s="2" t="inlineStr">
+        <is>
+          <t>Slide de abertura no padrão (roteiro + mensagem‑chave).</t>
+        </is>
+      </c>
+      <c r="I30" s="2" t="inlineStr">
+        <is>
+          <t>SBC 2025 (Dislipidemias/Prevenção) + MESA/SCOT-HEART (contexto)</t>
+        </is>
+      </c>
+      <c r="J30" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="inlineStr">
+        <is>
+          <t>GRADE</t>
+        </is>
+      </c>
+      <c r="B31" s="2" t="inlineStr">
+        <is>
+          <t>S61</t>
+        </is>
+      </c>
+      <c r="C31" s="2" t="inlineStr">
+        <is>
+          <t>Abertura do bloco ácido bempedóico</t>
+        </is>
+      </c>
+      <c r="D31" s="2" t="inlineStr">
+        <is>
+          <t>SBC 2025</t>
+        </is>
+      </c>
+      <c r="E31" s="3" t="inlineStr">
+        <is>
+          <t>Novo</t>
+        </is>
+      </c>
+      <c r="F31" s="3" t="inlineStr">
+        <is>
+          <t>P0</t>
+        </is>
+      </c>
+      <c r="G31" s="2" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="H31" s="2" t="inlineStr">
+        <is>
+          <t>Slide note + mensagem‑chave (diretriz → RCT → EtD/BR).</t>
+        </is>
+      </c>
+      <c r="I31" s="2" t="inlineStr">
+        <is>
+          <t>SBC 2025 + NEJM 2023 (CLEAR Outcomes)</t>
+        </is>
+      </c>
+      <c r="J31" s="2" t="inlineStr">
         <is>
           <t>-</t>
         </is>

</xml_diff>

<commit_message>
feat: OSTEOPOROSE viewer - melhor versÃ£o com correÃ§Ãµes de corte e fullscreen
- CorreÃ§Ãµes ortogrÃ¡ficas em S01, S02, S04, S05
- Ajustes de padding em S03, S07, S09 para evitar cortes
- Fullscreen mode: remove padding e oculta UI completamente
- fitSlideOverflow desabilitado temporariamente (abordagem CSS conservadora)
- print.css: ajustes mÃ­nimos de padding-bottom para casos extremos
- CorreÃ§Ã£o do contador de slides (72 slides corretos)
- PDF export: formato 16:9 correto via @page rule
- DocumentaÃ§Ã£o: OSTEOPOROSE_VIEWER_FIX_ATTEMPTS.md e PROMPT_CHATGPT_OSTEOPOROSE_FIX.md
- Script de export para ChatGPT: create-chatgpt-zip.ps1
- AtualizaÃ§Ã£o de CHANGELOG e README com histÃ³rico de tentativas
</commit_message>
<xml_diff>
--- a/DASHBOARD.xlsx
+++ b/DASHBOARD.xlsx
@@ -329,7 +329,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -429,7 +429,7 @@
       </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>P0</t>
+          <t>P1</t>
         </is>
       </c>
       <c r="G2" s="2" t="inlineStr">
@@ -439,12 +439,12 @@
       </c>
       <c r="H2" s="2" t="inlineStr">
         <is>
-          <t>Cards inferiores em paralelo + rodapé absoluto; placeholder KM (esquemático) pronto para substituir pela figura do paper.</t>
+          <t>Figura incluída (KM esquemático) + citação SCOT-HEART 10y corrigida; padding ajustado.</t>
         </is>
       </c>
       <c r="I2" s="2" t="inlineStr">
         <is>
-          <t>Lancet 2025 (SCOT-HEART 10y; 10.1016/S0140-6736(24)02679-5; CC BY 4.0); Circulation 2020 (LAP)</t>
+          <t>Lancet 2025 (SCOT-HEART 10y; 10.1016/S0140-6736(24)01899-5); Circulation 2020 (LAP)</t>
         </is>
       </c>
       <c r="J2" s="2" t="inlineStr">
@@ -684,7 +684,7 @@
       </c>
       <c r="E7" s="3" t="inlineStr">
         <is>
-          <t>Atualizado</t>
+          <t>Reposicionado</t>
         </is>
       </c>
       <c r="F7" s="3" t="inlineStr">
@@ -694,17 +694,17 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>2026-01-25</t>
+          <t>2026-01-23</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
         <is>
-          <t>Reservado espaço inferior + rodapé absoluto (evita corte em projeção).</t>
+          <t>Mantido conteúdo; reposicionado como ponte para EtD</t>
         </is>
       </c>
       <c r="I7" s="2" t="inlineStr">
         <is>
-          <t>NEJM 2023 (CLEAR Outcomes; 10.1056/NEJMoa2215024)</t>
+          <t>NEJM 2023 (CLEAR Outcomes)</t>
         </is>
       </c>
       <c r="J7" s="2" t="inlineStr">
@@ -1783,106 +1783,210 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="2" t="inlineStr">
-        <is>
-          <t>GRADE</t>
-        </is>
-      </c>
-      <c r="B30" s="2" t="inlineStr">
-        <is>
-          <t>S60</t>
-        </is>
-      </c>
-      <c r="C30" s="2" t="inlineStr">
-        <is>
-          <t>Abertura do bloco CAC</t>
-        </is>
-      </c>
-      <c r="D30" s="2" t="inlineStr">
-        <is>
-          <t>CAC / Evidência</t>
-        </is>
-      </c>
-      <c r="E30" s="3" t="inlineStr">
-        <is>
-          <t>Novo</t>
-        </is>
-      </c>
-      <c r="F30" s="3" t="inlineStr">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>OSTEOPOROSE</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>VIEWER</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Viewer: fit-to-screen + safe bottom</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Infra</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Atualizado</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
         <is>
           <t>P0</t>
         </is>
       </c>
-      <c r="G30" s="2" t="inlineStr">
-        <is>
-          <t>2026-01-25</t>
-        </is>
-      </c>
-      <c r="H30" s="2" t="inlineStr">
-        <is>
-          <t>Slide de abertura no padrão (roteiro + mensagem‑chave).</t>
-        </is>
-      </c>
-      <c r="I30" s="2" t="inlineStr">
-        <is>
-          <t>SBC 2025 (Dislipidemias/Prevenção) + MESA/SCOT-HEART (contexto)</t>
-        </is>
-      </c>
-      <c r="J30" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>2026-01-26</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>scheduleFit multi-pass + assets listeners + 100dvh</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>Validar em fullscreen/projetor</t>
         </is>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="2" t="inlineStr">
-        <is>
-          <t>GRADE</t>
-        </is>
-      </c>
-      <c r="B31" s="2" t="inlineStr">
-        <is>
-          <t>S61</t>
-        </is>
-      </c>
-      <c r="C31" s="2" t="inlineStr">
-        <is>
-          <t>Abertura do bloco ácido bempedóico</t>
-        </is>
-      </c>
-      <c r="D31" s="2" t="inlineStr">
-        <is>
-          <t>SBC 2025</t>
-        </is>
-      </c>
-      <c r="E31" s="3" t="inlineStr">
-        <is>
-          <t>Novo</t>
-        </is>
-      </c>
-      <c r="F31" s="3" t="inlineStr">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>OSTEOPOROSE</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>PRINT</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Print/PDF 16:9: sizing + fit</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Infra</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Atualizado</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
         <is>
           <t>P0</t>
         </is>
       </c>
-      <c r="G31" s="2" t="inlineStr">
-        <is>
-          <t>2026-01-25</t>
-        </is>
-      </c>
-      <c r="H31" s="2" t="inlineStr">
-        <is>
-          <t>Slide note + mensagem‑chave (diretriz → RCT → EtD/BR).</t>
-        </is>
-      </c>
-      <c r="I31" s="2" t="inlineStr">
-        <is>
-          <t>SBC 2025 + NEJM 2023 (CLEAR Outcomes)</t>
-        </is>
-      </c>
-      <c r="J31" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>2026-01-26</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>min-height override + print-fit.js + print.html regenerado</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>Re-testar export no Chrome/Edge</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>OSTEOPOROSE</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>S08</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>O que é Utilidade em Saúde?</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Utilidade/QALY</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Atualizado</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>2026-01-26</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>Redução de densidade + headings em navy (gold como acento)</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>Brazier 2002; Peasgood 2009</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>Checar se ainda precisa de fit</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>OSTEOPOROSE</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>S14</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Paradoxo: fraturas em osteopenia</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>FRAX / Conceitos</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Atualizado</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>P1</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>2026-01-26</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>Redução de densidade (padding/margens) + gráfico menor</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>Siris 2004</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>Checar legibilidade do gráfico em projeção</t>
         </is>
       </c>
     </row>
@@ -1897,7 +2001,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2015,6 +2119,33 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2026-01-26</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>OSTEOPOROSE_PATCH0_5</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Viewer fit (corte inferior) + Print/PDF 16:9 (min-height) + polish S08/S14</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>OSTEOPOROSE-changelog-dashboard_PATCH0_5.zip</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>P0: stage 100dvh + safe bottom; print-fit.js; print.html regenerado</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
docs: Documentar tentativas OSTEOPOROSE viewer/print/PDF (revertidas)
- CHANGELOG: SeÃ§Ã£o OSTEOPOROSE_TENTATIVAS_2026_01_27 com anÃ¡lise das 4 estratÃ©gias tentadas
- README: Nota sobre tentativas revertidas e prÃ³ximas estratÃ©gias sugeridas

Todas as alteraÃ§Ãµes de cÃ³digo foram revertidas para estado anterior.
Problemas identificados: conteÃºdo muito alto, fitSlideOverflow insuficiente, conflitos CSS print/viewer.
</commit_message>
<xml_diff>
--- a/DASHBOARD.xlsx
+++ b/DASHBOARD.xlsx
@@ -2001,7 +2001,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2146,6 +2146,33 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2026-01-27</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>OSTEOPOROSE_PATCH0_6</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Viewer: fit sem cortes (vh var + floor scale + translate/scale overflow). PDF: novo player full-screen + teclado. Print: print-fit mais robusto.</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>OSTEOPOROSE_PATCH0_6.zip</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>PDF em assets é placeholder; regenerar via print.html para 72 páginas 16:9.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>